<commit_message>
adds Consent Controls ; closes #115
- adds consent controls as a consent module
- controls: Obtain, Provide, Withdaw, Reaffirm
- moves properties from consent to legal basis: isIndicatedBy,
  hasIndicationMethod, isIndicatedAtTime
</commit_message>
<xml_diff>
--- a/code/vocab_csv/legal_basis.xlsx
+++ b/code/vocab_csv/legal_basis.xlsx
@@ -7,7 +7,8 @@
     <sheet state="visible" name="LegalBasis_properties" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="ConsentTypes" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="ConsentStatus" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Consent_properties" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="ConsentControls" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Consent_properties" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="291">
   <si>
     <t>Term</t>
   </si>
@@ -347,6 +348,42 @@
     <t>Axel Polleres, Javier Fernández</t>
   </si>
   <si>
+    <t>isIndicatedBy</t>
+  </si>
+  <si>
+    <t>is indicated by</t>
+  </si>
+  <si>
+    <t>Specifies entity who indicates the specific context</t>
+  </si>
+  <si>
+    <t>dpv:Entity</t>
+  </si>
+  <si>
+    <t>Georg P. Krog, Harshvardhan J. Pandit, Paul Ryan, Julian Flake</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/2022/06/22-dpvcg-minutes.html</t>
+  </si>
+  <si>
+    <t>hasIndicationMethod</t>
+  </si>
+  <si>
+    <t>has indication method</t>
+  </si>
+  <si>
+    <t>Specifies the method by which an entity has indicated the specific context</t>
+  </si>
+  <si>
+    <t>isIndicatedAtTime</t>
+  </si>
+  <si>
+    <t>is indicated at time</t>
+  </si>
+  <si>
+    <t>Specifies the temporal information for when the entity has indicated the specific context</t>
+  </si>
+  <si>
     <t>UninformedConsent</t>
   </si>
   <si>
@@ -357,12 +394,6 @@
   </si>
   <si>
     <t>dpv:Consent</t>
-  </si>
-  <si>
-    <t>Georg P. Krog, Harshvardhan J. Pandit, Paul Ryan, Julian Flake</t>
-  </si>
-  <si>
-    <t>https://www.w3.org/2022/06/22-dpvcg-minutes.html</t>
   </si>
   <si>
     <t>InformedConsent</t>
@@ -802,34 +833,70 @@
     </r>
   </si>
   <si>
-    <t>isIndicatedBy</t>
-  </si>
-  <si>
-    <t>is indicated by</t>
-  </si>
-  <si>
-    <t>Specifies entity who indicates the specific context</t>
-  </si>
-  <si>
-    <t>dpv:Entity</t>
-  </si>
-  <si>
-    <t>hasIndicationMethod</t>
-  </si>
-  <si>
-    <t>has indication method</t>
-  </si>
-  <si>
-    <t>Specifies the method by which an entity has indicated the specific context</t>
-  </si>
-  <si>
-    <t>isIndicatedAtTime</t>
-  </si>
-  <si>
-    <t>is indicated at time</t>
-  </si>
-  <si>
-    <t>Specifies the temporal information for when the entity has indicated the specific context</t>
+    <t>ConsentControl</t>
+  </si>
+  <si>
+    <t>The control or activity associated with obtaining, providing, withdrawing, or reaffirming consent</t>
+  </si>
+  <si>
+    <t>dpv:EntityInvolvement</t>
+  </si>
+  <si>
+    <t>ObtainConsent</t>
+  </si>
+  <si>
+    <t>Obtain Consent</t>
+  </si>
+  <si>
+    <t>Control for obtaining consent</t>
+  </si>
+  <si>
+    <t>dpv:ConsentControl</t>
+  </si>
+  <si>
+    <t>Indicates how the controller or entity can obtain consent e.g. used with dpv:isExercisedAt</t>
+  </si>
+  <si>
+    <t>ProvideConsent</t>
+  </si>
+  <si>
+    <t>Provide Consent</t>
+  </si>
+  <si>
+    <t>Control for providing consent</t>
+  </si>
+  <si>
+    <t>dpv:ConsentControl,dpv:OptingIntoProcess</t>
+  </si>
+  <si>
+    <t>Indicates how the data subject can provide consent e.g. used with dpv:isExercisedAt</t>
+  </si>
+  <si>
+    <t>WithdrawConsent</t>
+  </si>
+  <si>
+    <t>Withdraw Consent</t>
+  </si>
+  <si>
+    <t>Control for withdrawing consent</t>
+  </si>
+  <si>
+    <t>dpv:ConsentControl,dpv:WithdrawingFromProcess</t>
+  </si>
+  <si>
+    <t>Indicates how the data subject can withdraw consent e.g. used with dpv:isExercisedAt</t>
+  </si>
+  <si>
+    <t>ReaffirmConsent</t>
+  </si>
+  <si>
+    <t>Reaffirm Consent</t>
+  </si>
+  <si>
+    <t>Control for affirming consent</t>
+  </si>
+  <si>
+    <t>Indicates how the controller (with dpv:ObtainConsent) or data subject (with dpv:ProvideConsent) can reaffirm consent e.g. used with dpv:isExercisedAt</t>
   </si>
   <si>
     <t>hasConsentStatus</t>
@@ -839,6 +906,15 @@
   </si>
   <si>
     <t>Specifies the state or status of consent</t>
+  </si>
+  <si>
+    <t>hasConsentControl</t>
+  </si>
+  <si>
+    <t>has consent control</t>
+  </si>
+  <si>
+    <t>Specific a control associated with consent</t>
   </si>
   <si>
     <t xml:space="preserve">Deprecated </t>
@@ -1145,7 +1221,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1234,6 +1310,9 @@
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
@@ -1281,24 +1360,24 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFE06666"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF4CCCC"/>
           <bgColor rgb="FFF4CCCC"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9EAD3"/>
-          <bgColor rgb="FFD9EAD3"/>
         </patternFill>
       </fill>
       <border/>
@@ -1324,6 +1403,10 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -2834,26 +2917,184 @@
       <c r="AA2" s="20"/>
       <c r="AB2" s="20"/>
     </row>
+    <row r="3">
+      <c r="A3" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="22">
+        <v>44733.0</v>
+      </c>
+      <c r="L3" s="20"/>
+      <c r="M3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="O3" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="20"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="20"/>
+      <c r="Y3" s="20"/>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="22">
+        <v>44733.0</v>
+      </c>
+      <c r="L4" s="20"/>
+      <c r="M4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="O4" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="20"/>
+      <c r="W4" s="20"/>
+      <c r="X4" s="20"/>
+      <c r="Y4" s="20"/>
+      <c r="Z4" s="20"/>
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="20"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="22">
+        <v>44733.0</v>
+      </c>
+      <c r="L5" s="20"/>
+      <c r="M5" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="O5" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="20"/>
+      <c r="X5" s="20"/>
+      <c r="Y5" s="20"/>
+      <c r="Z5" s="20"/>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="20"/>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A3:AB5">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$M3="accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:AB5">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$M3="proposed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:AB5">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$M3="sunset"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A2:AB2">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$M2="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AB24">
-    <cfRule type="expression" dxfId="0" priority="2">
+  <conditionalFormatting sqref="A2:AB2 A6:AB24">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AB24">
-    <cfRule type="expression" dxfId="1" priority="3">
+  <conditionalFormatting sqref="A2:AB2 A6:AB24">
+    <cfRule type="expression" dxfId="1" priority="6">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="O2"/>
+    <hyperlink r:id="rId2" ref="O3"/>
+    <hyperlink r:id="rId3" ref="O4"/>
+    <hyperlink r:id="rId4" ref="O5"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -2919,16 +3160,16 @@
     </row>
     <row r="2">
       <c r="A2" s="18" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>25</v>
@@ -2967,16 +3208,16 @@
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>25</v>
@@ -2985,7 +3226,7 @@
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
       <c r="I3" s="18" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="J3" s="20"/>
       <c r="K3" s="22">
@@ -3017,16 +3258,16 @@
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>25</v>
@@ -3035,7 +3276,7 @@
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
       <c r="I4" s="18" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J4" s="20"/>
       <c r="K4" s="22">
@@ -3067,16 +3308,16 @@
     </row>
     <row r="5">
       <c r="A5" s="18" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>25</v>
@@ -3085,7 +3326,7 @@
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
       <c r="I5" s="18" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="J5" s="20"/>
       <c r="K5" s="22">
@@ -3117,16 +3358,16 @@
     </row>
     <row r="6">
       <c r="A6" s="18" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>25</v>
@@ -3135,7 +3376,7 @@
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
       <c r="I6" s="18" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="J6" s="20"/>
       <c r="K6" s="22">
@@ -3249,29 +3490,29 @@
     </row>
     <row r="2">
       <c r="A2" s="18" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="B2" s="18" t="str">
         <f>CONCATENATE(LEFT(A2,7)," ",RIGHT(A2,LEN(A2) - 7))</f>
         <v>Consent Status</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="18" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="J2" s="29" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="K2" s="22">
         <v>44734.0</v>
@@ -3302,26 +3543,26 @@
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="18" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
       <c r="I3" s="18" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="K3" s="22">
         <v>44734.0</v>
@@ -3352,26 +3593,26 @@
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="18" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
       <c r="I4" s="18" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="J4" s="29" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K4" s="22">
         <v>44734.0</v>
@@ -3402,29 +3643,29 @@
     </row>
     <row r="5">
       <c r="A5" s="18" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="B5" s="18" t="str">
         <f t="shared" ref="B5:B6" si="1">CONCATENATE(LEFT(A5,7)," ",RIGHT(A5,LEN(A5) - 7))</f>
         <v>Consent Unknown</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="D5" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>153</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>143</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
       <c r="I5" s="18" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="K5" s="22">
         <v>44734.0</v>
@@ -3455,29 +3696,29 @@
     </row>
     <row r="6">
       <c r="A6" s="18" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="B6" s="18" t="str">
         <f t="shared" si="1"/>
         <v>Consent Requested</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="D6" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>153</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>143</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
       <c r="I6" s="18" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="J6" s="29" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="K6" s="22">
         <v>44734.0</v>
@@ -3508,28 +3749,28 @@
     </row>
     <row r="7">
       <c r="A7" s="18" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="D7" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>153</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>143</v>
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
       <c r="I7" s="18" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="J7" s="29" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="K7" s="22">
         <v>44734.0</v>
@@ -3560,28 +3801,28 @@
     </row>
     <row r="8">
       <c r="A8" s="18" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="D8" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" s="18" t="s">
         <v>153</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>143</v>
       </c>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
       <c r="I8" s="18" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="J8" s="29" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="K8" s="22">
         <v>44734.0</v>
@@ -3612,28 +3853,28 @@
     </row>
     <row r="9">
       <c r="A9" s="18" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
       <c r="I9" s="18" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="J9" s="29" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="K9" s="22">
         <v>44734.0</v>
@@ -3664,28 +3905,28 @@
     </row>
     <row r="10">
       <c r="A10" s="18" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="D10" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E10" s="18" t="s">
         <v>153</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>143</v>
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
       <c r="I10" s="18" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="J10" s="29" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="K10" s="22">
         <v>44734.0</v>
@@ -3716,28 +3957,28 @@
     </row>
     <row r="11">
       <c r="A11" s="18" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="D11" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>153</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>143</v>
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
       <c r="I11" s="18" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="J11" s="29" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="K11" s="22">
         <v>44734.0</v>
@@ -3768,28 +4009,28 @@
     </row>
     <row r="12">
       <c r="A12" s="18" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="D12" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>153</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>143</v>
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
       <c r="I12" s="18" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="J12" s="29" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="K12" s="22">
         <v>44734.0</v>
@@ -3820,28 +4061,28 @@
     </row>
     <row r="13">
       <c r="A13" s="18" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="D13" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>153</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>143</v>
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
       <c r="I13" s="18" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="J13" s="29" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="K13" s="22">
         <v>44734.0</v>
@@ -3872,28 +4113,28 @@
     </row>
     <row r="14">
       <c r="A14" s="18" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
       <c r="I14" s="18" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="J14" s="29" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="K14" s="22">
         <v>44734.0</v>
@@ -3975,10 +4216,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="15.63"/>
-    <col customWidth="1" min="3" max="3" width="31.63"/>
-    <col customWidth="1" min="4" max="4" width="15.88"/>
-    <col customWidth="1" min="5" max="5" width="13.88"/>
+    <col customWidth="1" min="1" max="1" width="23.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.5" customHeight="1">
@@ -3992,13 +4230,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>103</v>
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -4006,14 +4244,14 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>104</v>
+        <v>10</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>11</v>
@@ -4030,38 +4268,35 @@
     </row>
     <row r="2">
       <c r="A2" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>202</v>
+        <v>211</v>
+      </c>
+      <c r="B2" s="18" t="str">
+        <f>CONCATENATE(LEFT(A2,7)," ",RIGHT(A2,LEN(A2) - 7))</f>
+        <v>Consent Control</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>18</v>
+        <v>213</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>204</v>
+        <v>147</v>
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
+      <c r="J2" s="30"/>
       <c r="K2" s="22">
-        <v>44733.0</v>
+        <v>45423.0</v>
       </c>
       <c r="L2" s="20"/>
       <c r="M2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="O2" s="23" t="s">
-        <v>115</v>
-      </c>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
       <c r="P2" s="20"/>
       <c r="Q2" s="20"/>
       <c r="R2" s="20"/>
@@ -4078,36 +4313,36 @@
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="20"/>
+        <v>217</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>147</v>
+      </c>
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
+      <c r="I3" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="J3" s="30"/>
       <c r="K3" s="22">
-        <v>44733.0</v>
+        <v>45423.0</v>
       </c>
       <c r="L3" s="20"/>
       <c r="M3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="O3" s="23" t="s">
-        <v>115</v>
-      </c>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
       <c r="P3" s="20"/>
       <c r="Q3" s="20"/>
       <c r="R3" s="20"/>
@@ -4124,36 +4359,36 @@
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="20"/>
+        <v>222</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>147</v>
+      </c>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="I4" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="J4" s="30"/>
       <c r="K4" s="22">
-        <v>44733.0</v>
+        <v>45423.0</v>
       </c>
       <c r="L4" s="20"/>
       <c r="M4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="O4" s="23" t="s">
-        <v>115</v>
-      </c>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
       <c r="P4" s="20"/>
       <c r="Q4" s="20"/>
       <c r="R4" s="20"/>
@@ -4170,38 +4405,36 @@
     </row>
     <row r="5">
       <c r="A5" s="18" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>18</v>
+        <v>227</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
+      <c r="I5" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="J5" s="30"/>
       <c r="K5" s="22">
-        <v>44733.0</v>
+        <v>45423.0</v>
       </c>
       <c r="L5" s="20"/>
       <c r="M5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="O5" s="23" t="s">
-        <v>115</v>
-      </c>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
       <c r="P5" s="20"/>
       <c r="Q5" s="20"/>
       <c r="R5" s="20"/>
@@ -4217,468 +4450,693 @@
       <c r="AB5" s="20"/>
     </row>
     <row r="6">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
+      <c r="A6" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="J6" s="30"/>
+      <c r="K6" s="22">
+        <v>45423.0</v>
+      </c>
+      <c r="L6" s="20"/>
+      <c r="M6" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20"/>
+      <c r="W6" s="20"/>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="20"/>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="20"/>
     </row>
     <row r="7">
-      <c r="A7" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="B7" s="18"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="22"/>
     </row>
     <row r="8">
-      <c r="A8" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="B8" s="30" t="s">
-        <v>216</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="K8" s="22">
-        <v>43560.0</v>
-      </c>
-      <c r="L8" s="22">
-        <v>44899.0</v>
-      </c>
-      <c r="M8" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N8" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="O8" s="23" t="s">
-        <v>115</v>
-      </c>
+      <c r="J8" s="30"/>
+      <c r="K8" s="22"/>
     </row>
     <row r="9">
-      <c r="A9" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>222</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="I9" s="25" t="s">
-        <v>218</v>
-      </c>
-      <c r="K9" s="22">
-        <v>43560.0</v>
-      </c>
-      <c r="L9" s="32">
-        <v>44899.0</v>
-      </c>
-      <c r="M9" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N9" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="O9" s="23" t="s">
-        <v>115</v>
-      </c>
+      <c r="J9" s="30"/>
+      <c r="K9" s="22"/>
     </row>
     <row r="10">
-      <c r="A10" s="18" t="s">
-        <v>225</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>226</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="I10" s="25" t="s">
-        <v>218</v>
-      </c>
-      <c r="K10" s="22">
-        <v>43560.0</v>
-      </c>
-      <c r="L10" s="22">
-        <v>44899.0</v>
-      </c>
-      <c r="M10" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N10" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="O10" s="23" t="s">
-        <v>115</v>
-      </c>
+      <c r="J10" s="30"/>
+      <c r="K10" s="22"/>
     </row>
     <row r="11">
-      <c r="A11" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>229</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="I11" s="33" t="s">
-        <v>231</v>
-      </c>
-      <c r="K11" s="22">
-        <v>43560.0</v>
-      </c>
-      <c r="L11" s="32">
-        <v>44899.0</v>
-      </c>
-      <c r="M11" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N11" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="O11" s="23" t="s">
-        <v>115</v>
-      </c>
+      <c r="J11" s="30"/>
+      <c r="K11" s="22"/>
     </row>
     <row r="12">
-      <c r="A12" s="18" t="s">
-        <v>232</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>233</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="K12" s="22">
-        <v>43560.0</v>
-      </c>
-      <c r="L12" s="22">
-        <v>44899.0</v>
-      </c>
-      <c r="M12" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N12" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="O12" s="23" t="s">
-        <v>115</v>
-      </c>
+      <c r="C12" s="25"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="22"/>
     </row>
     <row r="13">
-      <c r="A13" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="I13" s="33" t="s">
-        <v>231</v>
-      </c>
-      <c r="K13" s="22">
-        <v>43560.0</v>
-      </c>
-      <c r="L13" s="32">
-        <v>44899.0</v>
-      </c>
-      <c r="M13" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N13" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="O13" s="23" t="s">
-        <v>115</v>
-      </c>
+      <c r="J13" s="30"/>
+      <c r="K13" s="22"/>
     </row>
     <row r="14">
-      <c r="A14" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>240</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="K14" s="22">
-        <v>43560.0</v>
-      </c>
-      <c r="L14" s="22">
-        <v>44899.0</v>
-      </c>
-      <c r="M14" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N14" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="O14" s="23" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="18" t="s">
-        <v>242</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>243</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="K15" s="22">
-        <v>43560.0</v>
-      </c>
-      <c r="L15" s="32">
-        <v>44899.0</v>
-      </c>
-      <c r="M15" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N15" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="O15" s="23" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>248</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="I16" s="25" t="s">
-        <v>246</v>
-      </c>
-      <c r="K16" s="22">
-        <v>43560.0</v>
-      </c>
-      <c r="L16" s="22">
-        <v>44899.0</v>
-      </c>
-      <c r="M16" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N16" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="O16" s="23" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>251</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>252</v>
-      </c>
-      <c r="I17" s="34" t="s">
-        <v>253</v>
-      </c>
-      <c r="K17" s="22">
-        <v>43560.0</v>
-      </c>
-      <c r="L17" s="32">
-        <v>44899.0</v>
-      </c>
-      <c r="M17" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N17" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="O17" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
-      <c r="S17" s="35"/>
-      <c r="T17" s="35"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="35"/>
-      <c r="X17" s="35"/>
-      <c r="Y17" s="35"/>
-      <c r="Z17" s="35"/>
-      <c r="AA17" s="35"/>
-      <c r="AB17" s="35"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>255</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="I18" s="25" t="s">
-        <v>253</v>
-      </c>
-      <c r="K18" s="22">
-        <v>43560.0</v>
-      </c>
-      <c r="L18" s="22">
-        <v>44899.0</v>
-      </c>
-      <c r="M18" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N18" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="O18" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="35"/>
-      <c r="X18" s="35"/>
-      <c r="Y18" s="35"/>
-      <c r="Z18" s="35"/>
-      <c r="AA18" s="35"/>
-      <c r="AB18" s="35"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="B19" s="31" t="s">
-        <v>258</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>259</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="K19" s="22">
-        <v>43560.0</v>
-      </c>
-      <c r="L19" s="32">
-        <v>44899.0</v>
-      </c>
-      <c r="M19" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N19" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="O19" s="23" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>262</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>264</v>
-      </c>
-      <c r="I20" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="K20" s="22">
-        <v>43560.0</v>
-      </c>
-      <c r="L20" s="22">
-        <v>44899.0</v>
-      </c>
-      <c r="M20" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="N20" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="O20" s="23" t="s">
-        <v>115</v>
-      </c>
+      <c r="J14" s="30"/>
+      <c r="K14" s="22"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:AB20">
+  <conditionalFormatting sqref="A2:AB100">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AB20">
+  <conditionalFormatting sqref="A2:AB100">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AB88">
-    <cfRule type="expression" dxfId="3" priority="3">
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="2" width="15.63"/>
+    <col customWidth="1" min="3" max="3" width="31.63"/>
+    <col customWidth="1" min="4" max="4" width="15.88"/>
+    <col customWidth="1" min="5" max="5" width="13.88"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="28.5" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="22">
+        <v>44733.0</v>
+      </c>
+      <c r="L2" s="20"/>
+      <c r="M2" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="O2" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="K3" s="22">
+        <v>45423.0</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="B7" s="18"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="K8" s="22">
+        <v>43560.0</v>
+      </c>
+      <c r="L8" s="22">
+        <v>44899.0</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="N8" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="O8" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="K9" s="22">
+        <v>43560.0</v>
+      </c>
+      <c r="L9" s="33">
+        <v>44899.0</v>
+      </c>
+      <c r="M9" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="N9" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="O9" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>251</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="K10" s="22">
+        <v>43560.0</v>
+      </c>
+      <c r="L10" s="22">
+        <v>44899.0</v>
+      </c>
+      <c r="M10" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="N10" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="O10" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="I11" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="K11" s="22">
+        <v>43560.0</v>
+      </c>
+      <c r="L11" s="33">
+        <v>44899.0</v>
+      </c>
+      <c r="M11" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="N11" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="O11" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="K12" s="22">
+        <v>43560.0</v>
+      </c>
+      <c r="L12" s="22">
+        <v>44899.0</v>
+      </c>
+      <c r="M12" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="N12" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="O12" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="I13" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="K13" s="22">
+        <v>43560.0</v>
+      </c>
+      <c r="L13" s="33">
+        <v>44899.0</v>
+      </c>
+      <c r="M13" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="N13" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="O13" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="K14" s="22">
+        <v>43560.0</v>
+      </c>
+      <c r="L14" s="22">
+        <v>44899.0</v>
+      </c>
+      <c r="M14" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="N14" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="O14" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="K15" s="22">
+        <v>43560.0</v>
+      </c>
+      <c r="L15" s="33">
+        <v>44899.0</v>
+      </c>
+      <c r="M15" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="N15" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="O15" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>271</v>
+      </c>
+      <c r="K16" s="22">
+        <v>43560.0</v>
+      </c>
+      <c r="L16" s="22">
+        <v>44899.0</v>
+      </c>
+      <c r="M16" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="N16" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="O16" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="I17" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="K17" s="22">
+        <v>43560.0</v>
+      </c>
+      <c r="L17" s="33">
+        <v>44899.0</v>
+      </c>
+      <c r="M17" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="N17" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="O17" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="36"/>
+      <c r="U17" s="36"/>
+      <c r="V17" s="36"/>
+      <c r="W17" s="36"/>
+      <c r="X17" s="36"/>
+      <c r="Y17" s="36"/>
+      <c r="Z17" s="36"/>
+      <c r="AA17" s="36"/>
+      <c r="AB17" s="36"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>278</v>
+      </c>
+      <c r="K18" s="22">
+        <v>43560.0</v>
+      </c>
+      <c r="L18" s="22">
+        <v>44899.0</v>
+      </c>
+      <c r="M18" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="N18" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="O18" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="36"/>
+      <c r="U18" s="36"/>
+      <c r="V18" s="36"/>
+      <c r="W18" s="36"/>
+      <c r="X18" s="36"/>
+      <c r="Y18" s="36"/>
+      <c r="Z18" s="36"/>
+      <c r="AA18" s="36"/>
+      <c r="AB18" s="36"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="K19" s="22">
+        <v>43560.0</v>
+      </c>
+      <c r="L19" s="33">
+        <v>44899.0</v>
+      </c>
+      <c r="M19" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="N19" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="O19" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="K20" s="22">
+        <v>43560.0</v>
+      </c>
+      <c r="L20" s="22">
+        <v>44899.0</v>
+      </c>
+      <c r="M20" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="N20" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="O20" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:AB2 A6:AB20">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$M2="accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:AB2 A6:AB20">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$M2="proposed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:AB2 A6:AB88">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$M2="sunset"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="O2"/>
-    <hyperlink r:id="rId2" ref="O3"/>
-    <hyperlink r:id="rId3" ref="O4"/>
-    <hyperlink r:id="rId4" ref="O5"/>
-    <hyperlink r:id="rId5" ref="O8"/>
-    <hyperlink r:id="rId6" ref="O9"/>
-    <hyperlink r:id="rId7" ref="O10"/>
-    <hyperlink r:id="rId8" ref="O11"/>
-    <hyperlink r:id="rId9" ref="O12"/>
-    <hyperlink r:id="rId10" ref="O13"/>
-    <hyperlink r:id="rId11" ref="O14"/>
-    <hyperlink r:id="rId12" ref="O15"/>
-    <hyperlink r:id="rId13" ref="O16"/>
-    <hyperlink r:id="rId14" ref="O17"/>
-    <hyperlink r:id="rId15" ref="O18"/>
-    <hyperlink r:id="rId16" ref="O19"/>
-    <hyperlink r:id="rId17" ref="O20"/>
+    <hyperlink r:id="rId2" ref="O8"/>
+    <hyperlink r:id="rId3" ref="O9"/>
+    <hyperlink r:id="rId4" ref="O10"/>
+    <hyperlink r:id="rId5" ref="O11"/>
+    <hyperlink r:id="rId6" ref="O12"/>
+    <hyperlink r:id="rId7" ref="O13"/>
+    <hyperlink r:id="rId8" ref="O14"/>
+    <hyperlink r:id="rId9" ref="O15"/>
+    <hyperlink r:id="rId10" ref="O16"/>
+    <hyperlink r:id="rId11" ref="O17"/>
+    <hyperlink r:id="rId12" ref="O18"/>
+    <hyperlink r:id="rId13" ref="O19"/>
+    <hyperlink r:id="rId14" ref="O20"/>
   </hyperlinks>
-  <drawing r:id="rId18"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adds documentation for DPV legal basis module
- adds documentation with examples for legal basis module in DPV
- adds examples
- remove 'core' files in /dpv which were leftover from previous
  structure of the repository (core is now moved to /dpv/modules)
- fixes description of legal bases where 'specified processing' is replaced
  with either 'specified processing of data and technologies'; and the
  sentence start with 'Activities are ..." to represent generalised use
  of legal bases and the scope change in v2
</commit_message>
<xml_diff>
--- a/code/vocab_csv/legal_basis.xlsx
+++ b/code/vocab_csv/legal_basis.xlsx
@@ -90,7 +90,7 @@
     <t>Consent</t>
   </si>
   <si>
-    <t>Consent of the Data Subject for specified processing</t>
+    <t>Consent of the Data Subject for specified process or activity</t>
   </si>
   <si>
     <t>dpv:LegalBasis</t>
@@ -117,7 +117,7 @@
     <t>Data Subject Contract</t>
   </si>
   <si>
-    <t>Creation, completion, fulfilment, or performance of a contract, with the Data Controller and Data Subject as parties, and involving specified processing</t>
+    <t>Creation, completion, fulfilment, or performance of a contract, with the Data Controller and Data Subject as parties, and involving specified processing of data or technologies</t>
   </si>
   <si>
     <t>dpv:Contract</t>
@@ -129,7 +129,7 @@
     <t>Data Processor Contract</t>
   </si>
   <si>
-    <t>Creation, completion, fulfilment, or performance of a contract, with the Data Controller and Data Processor as parties, and involving specified processing</t>
+    <t>Creation, completion, fulfilment, or performance of a contract, with the Data Controller and Data Processor as parties, and involving specified processing of data or technologies</t>
   </si>
   <si>
     <t>DataControllerContract</t>
@@ -138,7 +138,7 @@
     <t>Data Controller Contract</t>
   </si>
   <si>
-    <t>Creation, completion, fulfilment, or performance of a contract, with Data Controllers as parties being Joint Data Controllers, and involving specified processing</t>
+    <t>Creation, completion, fulfilment, or performance of a contract, with Data Controllers as parties being Joint Data Controllers, and involving specified processing of data or technologies</t>
   </si>
   <si>
     <t>ThirdPartyContract</t>
@@ -147,7 +147,7 @@
     <t>Third Party Contract</t>
   </si>
   <si>
-    <t>Creation, completion, fulfilment, or performance of a contract, with the Data Controller and Third Party as parties, and involving specified processing</t>
+    <t>Creation, completion, fulfilment, or performance of a contract, with the Data Controller and Third Party as parties, and involving specified processing of data or technologies</t>
   </si>
   <si>
     <t>ContractPerformance</t>
@@ -156,7 +156,7 @@
     <t>Contract Performance</t>
   </si>
   <si>
-    <t>Fulfilment or performance of a contract involving specified processing</t>
+    <t>Fulfilment or performance of a contract involving specified processing of data or technologies</t>
   </si>
   <si>
     <t>Georg P. Krog, Harshvardhan J. Pandit, Paul Ryan</t>
@@ -192,7 +192,7 @@
     <t>Legal Obligation</t>
   </si>
   <si>
-    <t>Legal Obligation to conduct the specified processing</t>
+    <t>Legal Obligation to conduct the specified activities</t>
   </si>
   <si>
     <t>LegitimateInterest</t>
@@ -201,7 +201,7 @@
     <t>Legitimate Interest</t>
   </si>
   <si>
-    <t>Legitimate Interests of a Party as justification for specified processing</t>
+    <t>Legitimate Interests of a Party as justification for specified activities</t>
   </si>
   <si>
     <t>https://www.w3.org/2021/05/19-dpvcg-minutes.html</t>
@@ -213,7 +213,7 @@
     <t>Legitimate Interest of Controller</t>
   </si>
   <si>
-    <t>Legitimate Interests of a Data Controller in conducting specified processing</t>
+    <t>Legitimate Interests of a Data Controller in conducting specified activities</t>
   </si>
   <si>
     <t>dpv:LegitimateInterest</t>
@@ -225,7 +225,7 @@
     <t>Legitimate Interest of Third Party</t>
   </si>
   <si>
-    <t>Legitimate Interests of a Third Party in conducting specified processing</t>
+    <t>Legitimate Interests of a Third Party in conducting specified activities</t>
   </si>
   <si>
     <t>LegitimateInterestOfDataSubject</t>
@@ -234,7 +234,7 @@
     <t>Legitimate Interest of Data Subject</t>
   </si>
   <si>
-    <t>Legitimate Interests of the Data Subject in conducting specified processing</t>
+    <t>Legitimate Interests of the Data Subject in conducting specified activities</t>
   </si>
   <si>
     <t>Georg P. Krog</t>
@@ -246,7 +246,7 @@
     <t>Official Authority of Controller</t>
   </si>
   <si>
-    <t>Processing necessary or authorised through the official authority granted to or vested in the Data Controller</t>
+    <t>Activities are necessary or authorised through the official authority granted to or vested in the Data Controller</t>
   </si>
   <si>
     <t>https://www.w3.org/2021/05/05-dpvcg-minutes.html</t>
@@ -258,7 +258,7 @@
     <t>Public Interest</t>
   </si>
   <si>
-    <t>Processing is necessary or beneficial for interest of the public or society at large</t>
+    <t>Activities are necessary or beneficial for interest of the public or society at large</t>
   </si>
   <si>
     <t>https://www.w3.org/2021/04/21-dpvcg-minutes.html</t>
@@ -270,7 +270,7 @@
     <t>Vital Interest</t>
   </si>
   <si>
-    <t>Processing is necessary or required to protect vital interests of a data subject or other natural person</t>
+    <t>Activities are necessary or required to protect vital interests of a data subject or other natural person</t>
   </si>
   <si>
     <t>VitalInterestOfDataSubject</t>
@@ -279,7 +279,7 @@
     <t>Vital Interest of Data Subject</t>
   </si>
   <si>
-    <t>Processing is necessary or required to protect vital interests of a data subject</t>
+    <t>Activities are necessary or required to protect vital interests of a data subject</t>
   </si>
   <si>
     <t>dpv:VitalInterestOfNaturalPerson</t>
@@ -291,7 +291,7 @@
     <t>Vital Interest of Natural Person</t>
   </si>
   <si>
-    <t>Processing is necessary or required to protect vital interests of a natural person</t>
+    <t>Activities are necessary or required to protect vital interests of a natural person</t>
   </si>
   <si>
     <t>dpv:VitalInterest</t>

</xml_diff>

<commit_message>
DPV: adds examples and concepts
- added `dpv:ManageConsent` and `dpv:WithdrawConsent` as consent
  controls as they are needed e.g. in notices
- added examples for Notice (layer, icon) and Legal Basis (contract,
  consent, legitimate interests, official authority, public interest,
  and vital interest) and Processing (Profiling nad Tracking)
- added examples to HTML for DPV TOMs (Notice) and Legal Basis and
  Processing (Profiling and Tracking)
</commit_message>
<xml_diff>
--- a/code/vocab_csv/legal_basis.xlsx
+++ b/code/vocab_csv/legal_basis.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="639">
   <si>
     <t>Term</t>
   </si>
@@ -1923,6 +1923,30 @@
   </si>
   <si>
     <t>Indicates how the controller (with dpv:ObtainConsent) or data subject (with dpv:ProvideConsent) can reaffirm consent e.g. used with dpv:isExercisedAt</t>
+  </si>
+  <si>
+    <t>RefuseConsent</t>
+  </si>
+  <si>
+    <t>Refuse Consent</t>
+  </si>
+  <si>
+    <t>Control for refusing consent</t>
+  </si>
+  <si>
+    <t>ManageConsent</t>
+  </si>
+  <si>
+    <t>Manage Consent</t>
+  </si>
+  <si>
+    <t>Control for managing a given consent in terms of providing, reaffirming, or withdrawing it</t>
+  </si>
+  <si>
+    <t>dpv:ProvideConsent,dpv:WithdrawConsent,dpv:ReaffirmConsent</t>
+  </si>
+  <si>
+    <t>Indicates how the data subject can manage their consent in terms of providing it, or reaffirming or withdrawing a given consent. This concept is useful to represent a single location or interface where multiple controls are provided for consent</t>
   </si>
   <si>
     <t>hasConsentStatus</t>
@@ -4795,12 +4819,96 @@
       <c r="AB6" s="21"/>
     </row>
     <row r="7">
+      <c r="A7" s="17" t="s">
+        <v>573</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>574</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>575</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>557</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="23" t="s">
+        <v>572</v>
+      </c>
       <c r="J7" s="54"/>
-      <c r="K7" s="20"/>
+      <c r="K7" s="20">
+        <v>45643.0</v>
+      </c>
+      <c r="L7" s="21"/>
+      <c r="M7" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="21"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="21"/>
+      <c r="Y7" s="21"/>
+      <c r="Z7" s="21"/>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="21"/>
     </row>
     <row r="8">
+      <c r="A8" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>577</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>578</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>579</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="23" t="s">
+        <v>580</v>
+      </c>
       <c r="J8" s="54"/>
-      <c r="K8" s="20"/>
+      <c r="K8" s="20">
+        <v>45643.0</v>
+      </c>
+      <c r="L8" s="21"/>
+      <c r="M8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="21"/>
+      <c r="AA8" s="21"/>
+      <c r="AB8" s="21"/>
     </row>
     <row r="9">
       <c r="J9" s="54"/>
@@ -4907,13 +5015,13 @@
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>573</v>
+        <v>581</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>574</v>
+        <v>582</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>575</v>
+        <v>583</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>18</v>
@@ -4955,13 +5063,13 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>576</v>
+        <v>584</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>577</v>
+        <v>585</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>578</v>
+        <v>586</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>18</v>
@@ -4982,22 +5090,22 @@
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
-        <v>579</v>
+        <v>587</v>
       </c>
       <c r="B7" s="17"/>
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>580</v>
+        <v>588</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>581</v>
+        <v>589</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>582</v>
+        <v>590</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>583</v>
+        <v>591</v>
       </c>
       <c r="K8" s="20">
         <v>43560.0</v>
@@ -5006,10 +5114,10 @@
         <v>44899.0</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="N8" s="17" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="O8" s="22" t="s">
         <v>458</v>
@@ -5017,19 +5125,19 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>586</v>
+        <v>594</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>587</v>
+        <v>595</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>588</v>
+        <v>596</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>589</v>
+        <v>597</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>583</v>
+        <v>591</v>
       </c>
       <c r="K9" s="20">
         <v>43560.0</v>
@@ -5038,10 +5146,10 @@
         <v>44899.0</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="N9" s="17" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="O9" s="22" t="s">
         <v>458</v>
@@ -5049,19 +5157,19 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>590</v>
+        <v>598</v>
       </c>
       <c r="B10" s="56" t="s">
+        <v>599</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>600</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>597</v>
+      </c>
+      <c r="I10" s="23" t="s">
         <v>591</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>592</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>589</v>
-      </c>
-      <c r="I10" s="23" t="s">
-        <v>583</v>
       </c>
       <c r="K10" s="20">
         <v>43560.0</v>
@@ -5070,10 +5178,10 @@
         <v>44899.0</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="O10" s="22" t="s">
         <v>458</v>
@@ -5081,16 +5189,16 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>593</v>
+        <v>601</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>594</v>
+        <v>602</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="I11" s="58" t="s">
-        <v>596</v>
+        <v>604</v>
       </c>
       <c r="K11" s="20">
         <v>43560.0</v>
@@ -5099,10 +5207,10 @@
         <v>44899.0</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="N11" s="17" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="O11" s="22" t="s">
         <v>458</v>
@@ -5110,16 +5218,16 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>597</v>
+        <v>605</v>
       </c>
       <c r="B12" s="56" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>600</v>
+        <v>608</v>
       </c>
       <c r="K12" s="20">
         <v>43560.0</v>
@@ -5128,10 +5236,10 @@
         <v>44899.0</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="N12" s="17" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="O12" s="22" t="s">
         <v>458</v>
@@ -5139,16 +5247,16 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>601</v>
+        <v>609</v>
       </c>
       <c r="B13" s="56" t="s">
-        <v>602</v>
+        <v>610</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="I13" s="58" t="s">
-        <v>596</v>
+        <v>604</v>
       </c>
       <c r="K13" s="20">
         <v>43560.0</v>
@@ -5157,10 +5265,10 @@
         <v>44899.0</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="N13" s="17" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="O13" s="22" t="s">
         <v>458</v>
@@ -5168,16 +5276,16 @@
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>604</v>
+        <v>612</v>
       </c>
       <c r="B14" s="56" t="s">
-        <v>605</v>
+        <v>613</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>606</v>
+        <v>614</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>600</v>
+        <v>608</v>
       </c>
       <c r="K14" s="20">
         <v>43560.0</v>
@@ -5186,10 +5294,10 @@
         <v>44899.0</v>
       </c>
       <c r="M14" s="17" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="O14" s="22" t="s">
         <v>458</v>
@@ -5197,19 +5305,19 @@
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>607</v>
+        <v>615</v>
       </c>
       <c r="B15" s="56" t="s">
-        <v>608</v>
+        <v>616</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>609</v>
+        <v>617</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>610</v>
+        <v>618</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>611</v>
+        <v>619</v>
       </c>
       <c r="K15" s="20">
         <v>43560.0</v>
@@ -5218,10 +5326,10 @@
         <v>44899.0</v>
       </c>
       <c r="M15" s="17" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="N15" s="17" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="O15" s="22" t="s">
         <v>458</v>
@@ -5229,19 +5337,19 @@
     </row>
     <row r="16">
       <c r="A16" s="17" t="s">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="B16" s="56" t="s">
-        <v>613</v>
+        <v>621</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>610</v>
+        <v>618</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>611</v>
+        <v>619</v>
       </c>
       <c r="K16" s="20">
         <v>43560.0</v>
@@ -5250,10 +5358,10 @@
         <v>44899.0</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="N16" s="17" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="O16" s="22" t="s">
         <v>458</v>
@@ -5261,16 +5369,16 @@
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>615</v>
+        <v>623</v>
       </c>
       <c r="B17" s="56" t="s">
-        <v>616</v>
+        <v>624</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>617</v>
+        <v>625</v>
       </c>
       <c r="I17" s="59" t="s">
-        <v>618</v>
+        <v>626</v>
       </c>
       <c r="K17" s="20">
         <v>43560.0</v>
@@ -5279,10 +5387,10 @@
         <v>44899.0</v>
       </c>
       <c r="M17" s="17" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="N17" s="17" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="O17" s="22" t="s">
         <v>458</v>
@@ -5303,16 +5411,16 @@
     </row>
     <row r="18">
       <c r="A18" s="17" t="s">
-        <v>619</v>
+        <v>627</v>
       </c>
       <c r="B18" s="56" t="s">
-        <v>620</v>
+        <v>628</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>621</v>
+        <v>629</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>618</v>
+        <v>626</v>
       </c>
       <c r="K18" s="20">
         <v>43560.0</v>
@@ -5321,10 +5429,10 @@
         <v>44899.0</v>
       </c>
       <c r="M18" s="17" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="N18" s="17" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="O18" s="22" t="s">
         <v>458</v>
@@ -5345,16 +5453,16 @@
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>622</v>
+        <v>630</v>
       </c>
       <c r="B19" s="56" t="s">
-        <v>623</v>
+        <v>631</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>624</v>
+        <v>632</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>625</v>
+        <v>633</v>
       </c>
       <c r="K19" s="20">
         <v>43560.0</v>
@@ -5363,10 +5471,10 @@
         <v>44899.0</v>
       </c>
       <c r="M19" s="17" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="N19" s="17" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="O19" s="22" t="s">
         <v>458</v>
@@ -5374,19 +5482,19 @@
     </row>
     <row r="20">
       <c r="A20" s="17" t="s">
-        <v>626</v>
+        <v>634</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>627</v>
+        <v>635</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>628</v>
+        <v>636</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>629</v>
+        <v>637</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>630</v>
+        <v>638</v>
       </c>
       <c r="K20" s="20">
         <v>43560.0</v>
@@ -5395,10 +5503,10 @@
         <v>44899.0</v>
       </c>
       <c r="M20" s="17" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="N20" s="17" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="O20" s="22" t="s">
         <v>458</v>

</xml_diff>

<commit_message>
FIX: DPV, AI; Add HTML contents
- See https://w3id.org/dpv/meetings/meeting-2025-01-02 for context
- Add ai:hasTechnique and ai:hasCapability to AI: these were already present in
  the spreadsheet but were not being included in RDF and HTML due to errors in
  `vocab_management.py` where the properties entry was not included for core and
  data modules
- DPV Legal Basis module: Create concepts to represent contract accepted by 1
  party, N parties, and ALL parties
- FIX DPV Legal Basis module page - add status table for each basis section
- Add references to the GDPR concept e.g. Art.4-1
- Added content to AI, EU-GDPR HTML for documentation
</commit_message>
<xml_diff>
--- a/code/vocab_csv/legal_basis.xlsx
+++ b/code/vocab_csv/legal_basis.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="650">
   <si>
     <t>Term</t>
   </si>
@@ -663,7 +663,40 @@
     <t>Contract Accepted</t>
   </si>
   <si>
-    <t>Status indicating the contract has been accepted by all parties</t>
+    <t>Status indicating the contract has been accepted by some or all entities</t>
+  </si>
+  <si>
+    <t>Additional specialised concepts are provided and recommended to represent the common but contextual uses of the phrasing "contract accepted" for 1) indicate this party has accepted the contract - dpv:ContractAcceptedThisEntity; 2) indicate some parties have accepted it and others are yet to make a decision - dpv:ContractAcceptedSomeEntities; and 3) indicate all parties have accepted the contract - dpv:ContractAcceptedAllEntities</t>
+  </si>
+  <si>
+    <t>ContractAcceptedSomeEntities</t>
+  </si>
+  <si>
+    <t>Contract Accepted by Some Entities</t>
+  </si>
+  <si>
+    <t>Status indicating the contract has been accepted by some entities and others are in the process of making a decision</t>
+  </si>
+  <si>
+    <t>dpv:ContractAccepted</t>
+  </si>
+  <si>
+    <t>ContractedAcceptedAllEntities</t>
+  </si>
+  <si>
+    <t>Contract Accepted by All Entities</t>
+  </si>
+  <si>
+    <t>Status indicating the contract has been accepted by all entities who are a party to the contract - which means the contract is now in effect</t>
+  </si>
+  <si>
+    <t>ContractAcceptedThisEntity</t>
+  </si>
+  <si>
+    <t>Contract Accepted by This Entity</t>
+  </si>
+  <si>
+    <t>Status indicating the contract has been accepted by the specific entity in context</t>
   </si>
   <si>
     <t>ContractImplemented</t>
@@ -3813,14 +3846,14 @@
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>487</v>
+        <v>498</v>
       </c>
       <c r="B2" s="17" t="str">
         <f>CONCATENATE(LEFT(A2,7)," ",RIGHT(A2,LEN(A2) - 7))</f>
         <v>Consent Status</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>488</v>
+        <v>499</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>196</v>
@@ -3832,10 +3865,10 @@
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
       <c r="I2" s="17" t="s">
-        <v>489</v>
+        <v>500</v>
       </c>
       <c r="J2" s="53" t="s">
-        <v>490</v>
+        <v>501</v>
       </c>
       <c r="K2" s="20">
         <v>44734.0</v>
@@ -3845,10 +3878,10 @@
         <v>21</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O2" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
@@ -3866,26 +3899,26 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>491</v>
+        <v>502</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>492</v>
+        <v>503</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>493</v>
+        <v>504</v>
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="17" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
       <c r="I3" s="17" t="s">
-        <v>495</v>
+        <v>506</v>
       </c>
       <c r="J3" s="53" t="s">
-        <v>496</v>
+        <v>507</v>
       </c>
       <c r="K3" s="20">
         <v>44734.0</v>
@@ -3895,10 +3928,10 @@
         <v>21</v>
       </c>
       <c r="N3" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O3" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P3" s="21"/>
       <c r="Q3" s="21"/>
@@ -3916,26 +3949,26 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>497</v>
+        <v>508</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>498</v>
+        <v>509</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>499</v>
+        <v>510</v>
       </c>
       <c r="D4" s="21"/>
       <c r="E4" s="17" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
       <c r="H4" s="21"/>
       <c r="I4" s="17" t="s">
-        <v>500</v>
+        <v>511</v>
       </c>
       <c r="J4" s="53" t="s">
-        <v>501</v>
+        <v>512</v>
       </c>
       <c r="K4" s="20">
         <v>44734.0</v>
@@ -3945,10 +3978,10 @@
         <v>21</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O4" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P4" s="21"/>
       <c r="Q4" s="21"/>
@@ -3966,29 +3999,29 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>502</v>
+        <v>513</v>
       </c>
       <c r="B5" s="17" t="str">
         <f t="shared" ref="B5:B6" si="1">CONCATENATE(LEFT(A5,7)," ",RIGHT(A5,LEN(A5) - 7))</f>
         <v>Consent Unknown</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>503</v>
+        <v>514</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>504</v>
+        <v>515</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
       <c r="I5" s="17" t="s">
-        <v>505</v>
+        <v>516</v>
       </c>
       <c r="J5" s="53" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="K5" s="20">
         <v>44734.0</v>
@@ -3998,10 +4031,10 @@
         <v>21</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O5" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P5" s="21"/>
       <c r="Q5" s="21"/>
@@ -4019,29 +4052,29 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>507</v>
+        <v>518</v>
       </c>
       <c r="B6" s="17" t="str">
         <f t="shared" si="1"/>
         <v>Consent Requested</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>508</v>
+        <v>519</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>504</v>
+        <v>515</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
       <c r="I6" s="17" t="s">
-        <v>509</v>
+        <v>520</v>
       </c>
       <c r="J6" s="53" t="s">
-        <v>510</v>
+        <v>521</v>
       </c>
       <c r="K6" s="20">
         <v>44734.0</v>
@@ -4051,10 +4084,10 @@
         <v>21</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O6" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P6" s="21"/>
       <c r="Q6" s="21"/>
@@ -4072,28 +4105,28 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>511</v>
+        <v>522</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>512</v>
+        <v>523</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>513</v>
+        <v>524</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>504</v>
+        <v>515</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
       <c r="I7" s="17" t="s">
-        <v>514</v>
+        <v>525</v>
       </c>
       <c r="J7" s="53" t="s">
-        <v>515</v>
+        <v>526</v>
       </c>
       <c r="K7" s="20">
         <v>44734.0</v>
@@ -4103,10 +4136,10 @@
         <v>21</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O7" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P7" s="21"/>
       <c r="Q7" s="21"/>
@@ -4124,28 +4157,28 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>516</v>
+        <v>527</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>517</v>
+        <v>528</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>518</v>
+        <v>529</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>504</v>
+        <v>515</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="17" t="s">
-        <v>519</v>
+        <v>530</v>
       </c>
       <c r="J8" s="53" t="s">
-        <v>520</v>
+        <v>531</v>
       </c>
       <c r="K8" s="20">
         <v>44734.0</v>
@@ -4155,10 +4188,10 @@
         <v>21</v>
       </c>
       <c r="N8" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O8" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P8" s="21"/>
       <c r="Q8" s="21"/>
@@ -4176,28 +4209,28 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>521</v>
+        <v>532</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>522</v>
+        <v>533</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>523</v>
+        <v>534</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>524</v>
+        <v>535</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
       <c r="I9" s="17" t="s">
-        <v>525</v>
+        <v>536</v>
       </c>
       <c r="J9" s="53" t="s">
-        <v>526</v>
+        <v>537</v>
       </c>
       <c r="K9" s="20">
         <v>44734.0</v>
@@ -4207,10 +4240,10 @@
         <v>21</v>
       </c>
       <c r="N9" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O9" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P9" s="21"/>
       <c r="Q9" s="21"/>
@@ -4228,28 +4261,28 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>527</v>
+        <v>538</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>528</v>
+        <v>539</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>529</v>
+        <v>540</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>504</v>
+        <v>515</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="17" t="s">
-        <v>530</v>
+        <v>541</v>
       </c>
       <c r="J10" s="53" t="s">
-        <v>531</v>
+        <v>542</v>
       </c>
       <c r="K10" s="20">
         <v>44734.0</v>
@@ -4259,10 +4292,10 @@
         <v>21</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O10" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P10" s="21"/>
       <c r="Q10" s="21"/>
@@ -4280,28 +4313,28 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>532</v>
+        <v>543</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>533</v>
+        <v>544</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>534</v>
+        <v>545</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>504</v>
+        <v>515</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
       <c r="I11" s="17" t="s">
-        <v>535</v>
+        <v>546</v>
       </c>
       <c r="J11" s="53" t="s">
-        <v>536</v>
+        <v>547</v>
       </c>
       <c r="K11" s="20">
         <v>44734.0</v>
@@ -4311,10 +4344,10 @@
         <v>21</v>
       </c>
       <c r="N11" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O11" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P11" s="21"/>
       <c r="Q11" s="21"/>
@@ -4332,28 +4365,28 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>537</v>
+        <v>548</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>538</v>
+        <v>549</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>539</v>
+        <v>550</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>504</v>
+        <v>515</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
       <c r="I12" s="17" t="s">
-        <v>540</v>
+        <v>551</v>
       </c>
       <c r="J12" s="53" t="s">
-        <v>541</v>
+        <v>552</v>
       </c>
       <c r="K12" s="20">
         <v>44734.0</v>
@@ -4363,10 +4396,10 @@
         <v>21</v>
       </c>
       <c r="N12" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O12" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P12" s="21"/>
       <c r="Q12" s="21"/>
@@ -4384,28 +4417,28 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>542</v>
+        <v>553</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>543</v>
+        <v>554</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>544</v>
+        <v>555</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>504</v>
+        <v>515</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="17" t="s">
-        <v>545</v>
+        <v>556</v>
       </c>
       <c r="J13" s="53" t="s">
-        <v>546</v>
+        <v>557</v>
       </c>
       <c r="K13" s="20">
         <v>44734.0</v>
@@ -4415,10 +4448,10 @@
         <v>21</v>
       </c>
       <c r="N13" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O13" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P13" s="21"/>
       <c r="Q13" s="21"/>
@@ -4436,28 +4469,28 @@
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>547</v>
+        <v>558</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>548</v>
+        <v>559</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>549</v>
+        <v>560</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>524</v>
+        <v>535</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="17" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="J14" s="53" t="s">
-        <v>551</v>
+        <v>562</v>
       </c>
       <c r="K14" s="20">
         <v>44734.0</v>
@@ -4467,10 +4500,10 @@
         <v>21</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O14" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P14" s="21"/>
       <c r="Q14" s="21"/>
@@ -4591,17 +4624,17 @@
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>552</v>
+        <v>563</v>
       </c>
       <c r="B2" s="17" t="str">
         <f>CONCATENATE(LEFT(A2,7)," ",RIGHT(A2,LEN(A2) - 7))</f>
         <v>Consent Control</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>553</v>
+        <v>564</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>197</v>
@@ -4636,16 +4669,16 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>554</v>
+        <v>565</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>555</v>
+        <v>566</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>556</v>
+        <v>567</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>557</v>
+        <v>568</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>197</v>
@@ -4654,7 +4687,7 @@
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
       <c r="I3" s="17" t="s">
-        <v>558</v>
+        <v>569</v>
       </c>
       <c r="J3" s="54"/>
       <c r="K3" s="20">
@@ -4682,16 +4715,16 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>559</v>
+        <v>570</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>560</v>
+        <v>571</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>561</v>
+        <v>572</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>562</v>
+        <v>573</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>197</v>
@@ -4700,7 +4733,7 @@
       <c r="G4" s="21"/>
       <c r="H4" s="21"/>
       <c r="I4" s="23" t="s">
-        <v>563</v>
+        <v>574</v>
       </c>
       <c r="J4" s="54"/>
       <c r="K4" s="20">
@@ -4728,16 +4761,16 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>564</v>
+        <v>575</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>565</v>
+        <v>576</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>566</v>
+        <v>577</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>567</v>
+        <v>578</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>197</v>
@@ -4746,7 +4779,7 @@
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
       <c r="I5" s="23" t="s">
-        <v>568</v>
+        <v>579</v>
       </c>
       <c r="J5" s="54"/>
       <c r="K5" s="20">
@@ -4774,16 +4807,16 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>569</v>
+        <v>580</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>570</v>
+        <v>581</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>571</v>
+        <v>582</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>557</v>
+        <v>568</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>197</v>
@@ -4792,7 +4825,7 @@
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
       <c r="I6" s="23" t="s">
-        <v>572</v>
+        <v>583</v>
       </c>
       <c r="J6" s="54"/>
       <c r="K6" s="20">
@@ -4820,16 +4853,16 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>573</v>
+        <v>584</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>574</v>
+        <v>585</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>575</v>
+        <v>586</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>557</v>
+        <v>568</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>197</v>
@@ -4838,7 +4871,7 @@
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
       <c r="I7" s="23" t="s">
-        <v>572</v>
+        <v>583</v>
       </c>
       <c r="J7" s="54"/>
       <c r="K7" s="20">
@@ -4866,16 +4899,16 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>576</v>
+        <v>587</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>578</v>
+        <v>589</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>579</v>
+        <v>590</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>197</v>
@@ -4884,7 +4917,7 @@
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="23" t="s">
-        <v>580</v>
+        <v>591</v>
       </c>
       <c r="J8" s="54"/>
       <c r="K8" s="20">
@@ -4977,13 +5010,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>306</v>
+        <v>317</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>308</v>
+        <v>319</v>
       </c>
       <c r="G1" s="27" t="s">
         <v>6</v>
@@ -4998,7 +5031,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="30" t="s">
-        <v>309</v>
+        <v>320</v>
       </c>
       <c r="L1" s="31" t="s">
         <v>11</v>
@@ -5015,19 +5048,19 @@
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>581</v>
+        <v>592</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>582</v>
+        <v>593</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>583</v>
+        <v>594</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>18</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>494</v>
+        <v>505</v>
       </c>
       <c r="F2" s="21"/>
       <c r="G2" s="21"/>
@@ -5042,10 +5075,10 @@
         <v>21</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O2" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
@@ -5063,19 +5096,19 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>584</v>
+        <v>595</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>585</v>
+        <v>596</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>586</v>
+        <v>597</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>557</v>
+        <v>568</v>
       </c>
       <c r="K3" s="20">
         <v>45423.0</v>
@@ -5090,22 +5123,22 @@
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
-        <v>587</v>
+        <v>598</v>
       </c>
       <c r="B7" s="17"/>
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>588</v>
+        <v>599</v>
       </c>
       <c r="B8" s="55" t="s">
-        <v>589</v>
+        <v>600</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>590</v>
+        <v>601</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>591</v>
+        <v>602</v>
       </c>
       <c r="K8" s="20">
         <v>43560.0</v>
@@ -5114,30 +5147,30 @@
         <v>44899.0</v>
       </c>
       <c r="M8" s="17" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="N8" s="17" t="s">
-        <v>593</v>
+        <v>604</v>
       </c>
       <c r="O8" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>594</v>
+        <v>605</v>
       </c>
       <c r="B9" s="56" t="s">
-        <v>595</v>
+        <v>606</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>596</v>
+        <v>607</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>597</v>
+        <v>608</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>591</v>
+        <v>602</v>
       </c>
       <c r="K9" s="20">
         <v>43560.0</v>
@@ -5146,30 +5179,30 @@
         <v>44899.0</v>
       </c>
       <c r="M9" s="17" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="N9" s="17" t="s">
-        <v>593</v>
+        <v>604</v>
       </c>
       <c r="O9" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>598</v>
+        <v>609</v>
       </c>
       <c r="B10" s="56" t="s">
-        <v>599</v>
+        <v>610</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>600</v>
+        <v>611</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>597</v>
+        <v>608</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>591</v>
+        <v>602</v>
       </c>
       <c r="K10" s="20">
         <v>43560.0</v>
@@ -5178,27 +5211,27 @@
         <v>44899.0</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>593</v>
+        <v>604</v>
       </c>
       <c r="O10" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>601</v>
+        <v>612</v>
       </c>
       <c r="B11" s="56" t="s">
-        <v>602</v>
+        <v>613</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>603</v>
+        <v>614</v>
       </c>
       <c r="I11" s="58" t="s">
-        <v>604</v>
+        <v>615</v>
       </c>
       <c r="K11" s="20">
         <v>43560.0</v>
@@ -5207,27 +5240,27 @@
         <v>44899.0</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="N11" s="17" t="s">
-        <v>593</v>
+        <v>604</v>
       </c>
       <c r="O11" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>605</v>
+        <v>616</v>
       </c>
       <c r="B12" s="56" t="s">
-        <v>606</v>
+        <v>617</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>607</v>
+        <v>618</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>608</v>
+        <v>619</v>
       </c>
       <c r="K12" s="20">
         <v>43560.0</v>
@@ -5236,27 +5269,27 @@
         <v>44899.0</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="N12" s="17" t="s">
-        <v>593</v>
+        <v>604</v>
       </c>
       <c r="O12" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>609</v>
+        <v>620</v>
       </c>
       <c r="B13" s="56" t="s">
-        <v>610</v>
+        <v>621</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>611</v>
+        <v>622</v>
       </c>
       <c r="I13" s="58" t="s">
-        <v>604</v>
+        <v>615</v>
       </c>
       <c r="K13" s="20">
         <v>43560.0</v>
@@ -5265,27 +5298,27 @@
         <v>44899.0</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="N13" s="17" t="s">
-        <v>593</v>
+        <v>604</v>
       </c>
       <c r="O13" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>612</v>
+        <v>623</v>
       </c>
       <c r="B14" s="56" t="s">
-        <v>613</v>
+        <v>624</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>614</v>
+        <v>625</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>608</v>
+        <v>619</v>
       </c>
       <c r="K14" s="20">
         <v>43560.0</v>
@@ -5294,30 +5327,30 @@
         <v>44899.0</v>
       </c>
       <c r="M14" s="17" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>593</v>
+        <v>604</v>
       </c>
       <c r="O14" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>615</v>
+        <v>626</v>
       </c>
       <c r="B15" s="56" t="s">
-        <v>616</v>
+        <v>627</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>617</v>
+        <v>628</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>618</v>
+        <v>629</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>619</v>
+        <v>630</v>
       </c>
       <c r="K15" s="20">
         <v>43560.0</v>
@@ -5326,30 +5359,30 @@
         <v>44899.0</v>
       </c>
       <c r="M15" s="17" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="N15" s="17" t="s">
-        <v>593</v>
+        <v>604</v>
       </c>
       <c r="O15" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="17" t="s">
-        <v>620</v>
+        <v>631</v>
       </c>
       <c r="B16" s="56" t="s">
-        <v>621</v>
+        <v>632</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>622</v>
+        <v>633</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>618</v>
+        <v>629</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>619</v>
+        <v>630</v>
       </c>
       <c r="K16" s="20">
         <v>43560.0</v>
@@ -5358,27 +5391,27 @@
         <v>44899.0</v>
       </c>
       <c r="M16" s="17" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="N16" s="17" t="s">
-        <v>593</v>
+        <v>604</v>
       </c>
       <c r="O16" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>623</v>
+        <v>634</v>
       </c>
       <c r="B17" s="56" t="s">
-        <v>624</v>
+        <v>635</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>625</v>
+        <v>636</v>
       </c>
       <c r="I17" s="59" t="s">
-        <v>626</v>
+        <v>637</v>
       </c>
       <c r="K17" s="20">
         <v>43560.0</v>
@@ -5387,13 +5420,13 @@
         <v>44899.0</v>
       </c>
       <c r="M17" s="17" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="N17" s="17" t="s">
-        <v>593</v>
+        <v>604</v>
       </c>
       <c r="O17" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P17" s="60"/>
       <c r="Q17" s="60"/>
@@ -5411,16 +5444,16 @@
     </row>
     <row r="18">
       <c r="A18" s="17" t="s">
-        <v>627</v>
+        <v>638</v>
       </c>
       <c r="B18" s="56" t="s">
-        <v>628</v>
+        <v>639</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>629</v>
+        <v>640</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>626</v>
+        <v>637</v>
       </c>
       <c r="K18" s="20">
         <v>43560.0</v>
@@ -5429,13 +5462,13 @@
         <v>44899.0</v>
       </c>
       <c r="M18" s="17" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="N18" s="17" t="s">
-        <v>593</v>
+        <v>604</v>
       </c>
       <c r="O18" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P18" s="60"/>
       <c r="Q18" s="60"/>
@@ -5453,16 +5486,16 @@
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>630</v>
+        <v>641</v>
       </c>
       <c r="B19" s="56" t="s">
-        <v>631</v>
+        <v>642</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>632</v>
+        <v>643</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>633</v>
+        <v>644</v>
       </c>
       <c r="K19" s="20">
         <v>43560.0</v>
@@ -5471,30 +5504,30 @@
         <v>44899.0</v>
       </c>
       <c r="M19" s="17" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="N19" s="17" t="s">
-        <v>593</v>
+        <v>604</v>
       </c>
       <c r="O19" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="17" t="s">
-        <v>634</v>
+        <v>645</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>635</v>
+        <v>646</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>636</v>
+        <v>647</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>637</v>
+        <v>648</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>638</v>
+        <v>649</v>
       </c>
       <c r="K20" s="20">
         <v>43560.0</v>
@@ -5503,13 +5536,13 @@
         <v>44899.0</v>
       </c>
       <c r="M20" s="17" t="s">
-        <v>592</v>
+        <v>603</v>
       </c>
       <c r="N20" s="17" t="s">
-        <v>593</v>
+        <v>604</v>
       </c>
       <c r="O20" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>
@@ -7436,7 +7469,9 @@
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
+      <c r="I7" s="17" t="s">
+        <v>214</v>
+      </c>
       <c r="J7" s="21"/>
       <c r="K7" s="20">
         <v>45531.0</v>
@@ -7464,15 +7499,17 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="D8" s="21"/>
+        <v>217</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>218</v>
+      </c>
       <c r="E8" s="17" t="s">
         <v>201</v>
       </c>
@@ -7482,7 +7519,7 @@
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
       <c r="K8" s="20">
-        <v>45531.0</v>
+        <v>45659.0</v>
       </c>
       <c r="L8" s="21"/>
       <c r="M8" s="17" t="s">
@@ -7507,15 +7544,17 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="D9" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="D9" s="21"/>
       <c r="E9" s="17" t="s">
         <v>201</v>
       </c>
@@ -7525,7 +7564,7 @@
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
       <c r="K9" s="20">
-        <v>45531.0</v>
+        <v>45659.0</v>
       </c>
       <c r="L9" s="21"/>
       <c r="M9" s="17" t="s">
@@ -7550,15 +7589,17 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="D10" s="21"/>
+        <v>224</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>218</v>
+      </c>
       <c r="E10" s="17" t="s">
         <v>201</v>
       </c>
@@ -7568,7 +7609,7 @@
       <c r="I10" s="21"/>
       <c r="J10" s="21"/>
       <c r="K10" s="20">
-        <v>45531.0</v>
+        <v>45659.0</v>
       </c>
       <c r="L10" s="21"/>
       <c r="M10" s="17" t="s">
@@ -7593,13 +7634,13 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="17" t="s">
@@ -7636,13 +7677,13 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="17" t="s">
@@ -7679,13 +7720,13 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="17" t="s">
@@ -7721,14 +7762,14 @@
       <c r="AC13" s="21"/>
     </row>
     <row r="14">
-      <c r="A14" s="8" t="s">
-        <v>232</v>
+      <c r="A14" s="17" t="s">
+        <v>234</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="17" t="s">
@@ -7765,17 +7806,15 @@
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>238</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="D15" s="21"/>
       <c r="E15" s="17" t="s">
         <v>201</v>
       </c>
@@ -7810,17 +7849,15 @@
     </row>
     <row r="16">
       <c r="A16" s="17" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>241</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>238</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="D16" s="21"/>
       <c r="E16" s="17" t="s">
         <v>201</v>
       </c>
@@ -7854,22 +7891,20 @@
       <c r="AC16" s="21"/>
     </row>
     <row r="17">
-      <c r="A17" s="17" t="s">
-        <v>242</v>
+      <c r="A17" s="8" t="s">
+        <v>243</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>244</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>238</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="D17" s="21"/>
       <c r="E17" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="F17" s="8"/>
+      <c r="F17" s="21"/>
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>
@@ -7898,13 +7933,148 @@
       <c r="AB17" s="21"/>
       <c r="AC17" s="21"/>
     </row>
+    <row r="18">
+      <c r="A18" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="20">
+        <v>45531.0</v>
+      </c>
+      <c r="L18" s="21"/>
+      <c r="M18" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="21"/>
+      <c r="U18" s="21"/>
+      <c r="V18" s="21"/>
+      <c r="W18" s="21"/>
+      <c r="X18" s="21"/>
+      <c r="Y18" s="21"/>
+      <c r="Z18" s="21"/>
+      <c r="AA18" s="21"/>
+      <c r="AB18" s="21"/>
+      <c r="AC18" s="21"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="20">
+        <v>45531.0</v>
+      </c>
+      <c r="L19" s="21"/>
+      <c r="M19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="21"/>
+      <c r="U19" s="21"/>
+      <c r="V19" s="21"/>
+      <c r="W19" s="21"/>
+      <c r="X19" s="21"/>
+      <c r="Y19" s="21"/>
+      <c r="Z19" s="21"/>
+      <c r="AA19" s="21"/>
+      <c r="AB19" s="21"/>
+      <c r="AC19" s="21"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="F20" s="8"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="20">
+        <v>45531.0</v>
+      </c>
+      <c r="L20" s="21"/>
+      <c r="M20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="21"/>
+      <c r="V20" s="21"/>
+      <c r="W20" s="21"/>
+      <c r="X20" s="21"/>
+      <c r="Y20" s="21"/>
+      <c r="Z20" s="21"/>
+      <c r="AA20" s="21"/>
+      <c r="AB20" s="21"/>
+      <c r="AC20" s="21"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:AF17 A22:AF213">
+  <conditionalFormatting sqref="A2:AF20 A25:AF216">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AC17 A22:AC52">
+  <conditionalFormatting sqref="A2:AC20 A25:AC55">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>$M2="accepted"</formula>
     </cfRule>
@@ -7976,13 +8146,13 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>18</v>
@@ -8021,17 +8191,17 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="17" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
@@ -8064,17 +8234,17 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="D4" s="21"/>
       <c r="E4" s="17" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
@@ -8107,17 +8277,17 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="17" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
@@ -8150,17 +8320,17 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="17" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
@@ -8193,17 +8363,17 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>262</v>
+        <v>273</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="17" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
@@ -8236,17 +8406,17 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="17" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
@@ -8279,17 +8449,17 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>269</v>
+        <v>280</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="17" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
@@ -8322,17 +8492,17 @@
     </row>
     <row r="10">
       <c r="A10" s="47" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="B10" s="47" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="17" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="F10" s="49"/>
       <c r="G10" s="49"/>
@@ -8378,13 +8548,13 @@
     </row>
     <row r="12">
       <c r="A12" s="8" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>274</v>
+        <v>285</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="17" t="s">
@@ -8421,16 +8591,16 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>276</v>
+        <v>287</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>278</v>
+        <v>289</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>279</v>
+        <v>290</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>201</v>
@@ -8466,16 +8636,16 @@
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>279</v>
+        <v>290</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>201</v>
@@ -8511,16 +8681,16 @@
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>279</v>
+        <v>290</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>201</v>
@@ -8642,16 +8812,16 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>197</v>
@@ -8687,16 +8857,16 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>197</v>
@@ -8732,16 +8902,16 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>295</v>
+        <v>306</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>197</v>
@@ -8777,16 +8947,16 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>298</v>
+        <v>309</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>197</v>
@@ -8822,16 +8992,16 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>301</v>
+        <v>312</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>197</v>
@@ -8867,16 +9037,16 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>316</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>304</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>305</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>293</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>197</v>
@@ -8949,13 +9119,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>306</v>
+        <v>317</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>308</v>
+        <v>319</v>
       </c>
       <c r="G1" s="27" t="s">
         <v>6</v>
@@ -8970,7 +9140,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="30" t="s">
-        <v>309</v>
+        <v>320</v>
       </c>
       <c r="L1" s="31" t="s">
         <v>11</v>
@@ -8987,55 +9157,55 @@
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>310</v>
+        <v>321</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>311</v>
+        <v>322</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>312</v>
+        <v>323</v>
       </c>
       <c r="E2" s="18"/>
       <c r="K2" s="20"/>
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>313</v>
+        <v>324</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>315</v>
+        <v>326</v>
       </c>
       <c r="E3" s="18"/>
       <c r="K3" s="20"/>
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>317</v>
+        <v>328</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="E4" s="18"/>
       <c r="I4" s="17" t="s">
-        <v>319</v>
+        <v>330</v>
       </c>
       <c r="K4" s="20"/>
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>320</v>
+        <v>331</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>321</v>
+        <v>332</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>322</v>
+        <v>333</v>
       </c>
       <c r="E5" s="18"/>
       <c r="I5" s="17"/>
@@ -9043,150 +9213,150 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>324</v>
+        <v>335</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>325</v>
+        <v>336</v>
       </c>
       <c r="E6" s="18"/>
       <c r="I6" s="17" t="s">
-        <v>326</v>
+        <v>337</v>
       </c>
       <c r="K6" s="20"/>
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>328</v>
+        <v>339</v>
       </c>
       <c r="E7" s="23"/>
       <c r="I7" s="17"/>
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>329</v>
+        <v>340</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>330</v>
+        <v>341</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="E8" s="23"/>
       <c r="I8" s="17" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>333</v>
+        <v>344</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>334</v>
+        <v>345</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>335</v>
+        <v>346</v>
       </c>
       <c r="E9" s="23"/>
       <c r="I9" s="17" t="s">
-        <v>336</v>
+        <v>347</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>337</v>
+        <v>348</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>342</v>
+        <v>353</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>345</v>
+        <v>356</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>347</v>
+        <v>358</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>348</v>
+        <v>359</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>352</v>
+        <v>363</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>353</v>
+        <v>364</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>354</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>355</v>
+        <v>366</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>358</v>
+        <v>369</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>359</v>
+        <v>370</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>360</v>
+        <v>371</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>361</v>
+        <v>372</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>34</v>
@@ -9195,7 +9365,7 @@
         <v>201</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>362</v>
+        <v>373</v>
       </c>
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
@@ -9227,22 +9397,22 @@
     </row>
     <row r="18">
       <c r="A18" s="17" t="s">
-        <v>363</v>
+        <v>374</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>364</v>
+        <v>375</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>201</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>367</v>
+        <v>378</v>
       </c>
       <c r="K18" s="20">
         <v>45531.0</v>
@@ -9254,19 +9424,19 @@
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>34</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
       <c r="K19" s="20">
         <v>45531.0</v>
@@ -9281,19 +9451,19 @@
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>371</v>
+        <v>382</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>372</v>
+        <v>383</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>373</v>
+        <v>384</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="K21" s="20">
         <v>45643.0</v>
@@ -9390,13 +9560,13 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="s">
-        <v>374</v>
+        <v>385</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>375</v>
+        <v>386</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>376</v>
+        <v>387</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>196</v>
@@ -9438,17 +9608,17 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>377</v>
+        <v>388</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>378</v>
+        <v>389</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>379</v>
+        <v>390</v>
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="17" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
@@ -9484,17 +9654,17 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>381</v>
+        <v>392</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>382</v>
+        <v>393</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>383</v>
+        <v>394</v>
       </c>
       <c r="D4" s="21"/>
       <c r="E4" s="17" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
@@ -9530,17 +9700,17 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>384</v>
+        <v>395</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>385</v>
+        <v>396</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>386</v>
+        <v>397</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="17" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
@@ -9576,17 +9746,17 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>387</v>
+        <v>398</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>388</v>
+        <v>399</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>389</v>
+        <v>400</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="17" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
@@ -9622,13 +9792,13 @@
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
-        <v>390</v>
+        <v>401</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>391</v>
+        <v>402</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>392</v>
+        <v>403</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>196</v>
@@ -9670,17 +9840,17 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>393</v>
+        <v>404</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>394</v>
+        <v>405</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>395</v>
+        <v>406</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="17" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
@@ -9716,17 +9886,17 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>397</v>
+        <v>408</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>398</v>
+        <v>409</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>399</v>
+        <v>410</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="17" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
@@ -9762,17 +9932,17 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>400</v>
+        <v>411</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>401</v>
+        <v>412</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>402</v>
+        <v>413</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="17" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
@@ -9808,13 +9978,13 @@
     </row>
     <row r="11">
       <c r="A11" s="8" t="s">
-        <v>403</v>
+        <v>414</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>404</v>
+        <v>415</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>405</v>
+        <v>416</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>196</v>
@@ -9856,16 +10026,16 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>406</v>
+        <v>417</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>407</v>
+        <v>418</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>408</v>
+        <v>419</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>409</v>
+        <v>420</v>
       </c>
       <c r="K12" s="20">
         <v>45531.0</v>
@@ -9896,17 +10066,17 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>410</v>
+        <v>421</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>411</v>
+        <v>422</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>412</v>
+        <v>423</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="17" t="s">
-        <v>409</v>
+        <v>420</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
@@ -9942,17 +10112,17 @@
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>413</v>
+        <v>424</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>414</v>
+        <v>425</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>415</v>
+        <v>426</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="17" t="s">
-        <v>409</v>
+        <v>420</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
@@ -9988,13 +10158,13 @@
     </row>
     <row r="15">
       <c r="A15" s="8" t="s">
-        <v>416</v>
+        <v>427</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>418</v>
+        <v>429</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>196</v>
@@ -10036,17 +10206,17 @@
     </row>
     <row r="16">
       <c r="A16" s="17" t="s">
-        <v>419</v>
+        <v>430</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>420</v>
+        <v>431</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>421</v>
+        <v>432</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="17" t="s">
-        <v>422</v>
+        <v>433</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="21"/>
@@ -10082,17 +10252,17 @@
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>424</v>
+        <v>435</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>425</v>
+        <v>436</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="17" t="s">
-        <v>422</v>
+        <v>433</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
@@ -10128,17 +10298,17 @@
     </row>
     <row r="18">
       <c r="A18" s="17" t="s">
-        <v>426</v>
+        <v>437</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>427</v>
+        <v>438</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>428</v>
+        <v>439</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="17" t="s">
-        <v>422</v>
+        <v>433</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="21"/>
@@ -10174,17 +10344,17 @@
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>429</v>
+        <v>440</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>430</v>
+        <v>441</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>431</v>
+        <v>442</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="17" t="s">
-        <v>422</v>
+        <v>433</v>
       </c>
       <c r="F19" s="21"/>
       <c r="G19" s="21"/>
@@ -10220,13 +10390,13 @@
     </row>
     <row r="20">
       <c r="A20" s="8" t="s">
-        <v>432</v>
+        <v>443</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>433</v>
+        <v>444</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>434</v>
+        <v>445</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>196</v>
@@ -10268,17 +10438,17 @@
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>435</v>
+        <v>446</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>436</v>
+        <v>447</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>437</v>
+        <v>448</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="17" t="s">
-        <v>438</v>
+        <v>449</v>
       </c>
       <c r="F21" s="21"/>
       <c r="G21" s="21"/>
@@ -10314,17 +10484,17 @@
     </row>
     <row r="22">
       <c r="A22" s="17" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>440</v>
+        <v>451</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>441</v>
+        <v>452</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="17" t="s">
-        <v>438</v>
+        <v>449</v>
       </c>
       <c r="F22" s="21"/>
       <c r="G22" s="21"/>
@@ -10360,17 +10530,17 @@
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>442</v>
+        <v>453</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>443</v>
+        <v>454</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>444</v>
+        <v>455</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="17" t="s">
-        <v>438</v>
+        <v>449</v>
       </c>
       <c r="F23" s="21"/>
       <c r="G23" s="21"/>
@@ -10406,17 +10576,17 @@
     </row>
     <row r="24">
       <c r="A24" s="17" t="s">
-        <v>445</v>
+        <v>456</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>446</v>
+        <v>457</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>447</v>
+        <v>458</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="17" t="s">
-        <v>438</v>
+        <v>449</v>
       </c>
       <c r="F24" s="21"/>
       <c r="G24" s="21"/>
@@ -10513,13 +10683,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>306</v>
+        <v>317</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>308</v>
+        <v>319</v>
       </c>
       <c r="G1" s="27" t="s">
         <v>6</v>
@@ -10534,7 +10704,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="30" t="s">
-        <v>309</v>
+        <v>320</v>
       </c>
       <c r="L1" s="31" t="s">
         <v>11</v>
@@ -10551,13 +10721,13 @@
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>448</v>
+        <v>459</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>449</v>
+        <v>460</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>450</v>
+        <v>461</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>18</v>
@@ -10567,7 +10737,7 @@
         <v>dpv:LegalBasis</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>451</v>
+        <v>462</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
@@ -10583,7 +10753,7 @@
         <v>21</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>452</v>
+        <v>463</v>
       </c>
       <c r="O2" s="22" t="s">
         <v>22</v>
@@ -10608,19 +10778,19 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>453</v>
+        <v>464</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>454</v>
+        <v>465</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>455</v>
+        <v>466</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>456</v>
+        <v>467</v>
       </c>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
@@ -10635,10 +10805,10 @@
         <v>21</v>
       </c>
       <c r="N3" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O3" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P3" s="21"/>
       <c r="Q3" s="21"/>
@@ -10660,13 +10830,13 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>459</v>
+        <v>470</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>460</v>
+        <v>471</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>461</v>
+        <v>472</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>18</v>
@@ -10685,10 +10855,10 @@
         <v>21</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O4" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P4" s="21"/>
       <c r="Q4" s="21"/>
@@ -10710,13 +10880,13 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>462</v>
+        <v>473</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>463</v>
+        <v>474</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>464</v>
+        <v>475</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>18</v>
@@ -10735,10 +10905,10 @@
         <v>21</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O5" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P5" s="21"/>
       <c r="Q5" s="21"/>
@@ -10907,16 +11077,16 @@
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>465</v>
+        <v>476</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>466</v>
+        <v>477</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>467</v>
+        <v>478</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>468</v>
+        <v>479</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>25</v>
@@ -10934,10 +11104,10 @@
         <v>21</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O2" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P2" s="21"/>
       <c r="Q2" s="21"/>
@@ -10955,16 +11125,16 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>469</v>
+        <v>480</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>470</v>
+        <v>481</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>471</v>
+        <v>482</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>468</v>
+        <v>479</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>25</v>
@@ -10973,7 +11143,7 @@
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
       <c r="I3" s="17" t="s">
-        <v>472</v>
+        <v>483</v>
       </c>
       <c r="J3" s="21"/>
       <c r="K3" s="20">
@@ -10984,10 +11154,10 @@
         <v>21</v>
       </c>
       <c r="N3" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O3" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P3" s="21"/>
       <c r="Q3" s="21"/>
@@ -11005,16 +11175,16 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>473</v>
+        <v>484</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>474</v>
+        <v>485</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>475</v>
+        <v>486</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>476</v>
+        <v>487</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>25</v>
@@ -11023,7 +11193,7 @@
       <c r="G4" s="21"/>
       <c r="H4" s="21"/>
       <c r="I4" s="17" t="s">
-        <v>477</v>
+        <v>488</v>
       </c>
       <c r="J4" s="21"/>
       <c r="K4" s="20">
@@ -11034,10 +11204,10 @@
         <v>21</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O4" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P4" s="21"/>
       <c r="Q4" s="21"/>
@@ -11055,16 +11225,16 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>478</v>
+        <v>489</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>479</v>
+        <v>490</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>480</v>
+        <v>491</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>476</v>
+        <v>487</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>25</v>
@@ -11073,7 +11243,7 @@
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
       <c r="I5" s="17" t="s">
-        <v>481</v>
+        <v>492</v>
       </c>
       <c r="J5" s="21"/>
       <c r="K5" s="20">
@@ -11084,10 +11254,10 @@
         <v>21</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O5" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P5" s="21"/>
       <c r="Q5" s="21"/>
@@ -11105,16 +11275,16 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>482</v>
+        <v>493</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>483</v>
+        <v>494</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>484</v>
+        <v>495</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>485</v>
+        <v>496</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>25</v>
@@ -11123,7 +11293,7 @@
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
       <c r="I6" s="17" t="s">
-        <v>486</v>
+        <v>497</v>
       </c>
       <c r="J6" s="21"/>
       <c r="K6" s="20">
@@ -11134,10 +11304,10 @@
         <v>21</v>
       </c>
       <c r="N6" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="O6" s="22" t="s">
-        <v>458</v>
+        <v>469</v>
       </c>
       <c r="P6" s="21"/>
       <c r="Q6" s="21"/>

</xml_diff>